<commit_message>
Açoes de botos adicionadas e titulo da tabela de acordo com o grafico
</commit_message>
<xml_diff>
--- a/homicidiosMulheresNegrasPais.xlsx
+++ b/homicidiosMulheresNegrasPais.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zsg-k\IdeaProjects\Excel-Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zsg-k\IdeaProjects\guiExample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A0047B-7D53-4C9C-AF10-FCEECFDCD42C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542BB0D4-E331-435A-97C2-F0C1C4F98BB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,17 +30,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.00_);\(0.00\)"/>
+    <numFmt numFmtId="164" formatCode="0.00_);\(0.00\)"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -554,7 +550,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,12 +561,16 @@
     <xf numFmtId="39" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -634,6 +634,42 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="7" formatCode="#,##0.00_);\(#,##0.00\)"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -823,42 +859,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="3"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="7" formatCode="#,##0.00_);\(#,##0.00\)"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -944,7 +944,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="#,##0.00;\-#,##0.00"/>
+      <numFmt numFmtId="165" formatCode="#,##0.00;\-#,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1153,10 +1153,10 @@
     <tableColumn id="2" xr3:uid="{0367045E-A6E2-4ADB-B386-F01A25A90280}" name="Valor" headerRowDxfId="13" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{B7C9F687-C2C9-48A0-8191-90F777E13E77}" name="Média Aritmética" headerRowDxfId="11" dataDxfId="10" dataCellStyle="Título 3"/>
     <tableColumn id="4" xr3:uid="{7EFBA212-C5D7-49CA-BA07-8F123C782962}" name="Desvio Médio" headerRowDxfId="9" dataDxfId="8" dataCellStyle="Título 3"/>
-    <tableColumn id="5" xr3:uid="{CA7852E6-72C8-4A1E-95CB-43E78C3FC0C2}" name="Desvio Padrão" headerRowDxfId="7" dataDxfId="6" dataCellStyle="Título 3"/>
-    <tableColumn id="6" xr3:uid="{27646C93-0C02-40E2-85AE-D3CFA65AB91D}" name="Variância Populacional" headerRowDxfId="5" dataDxfId="4" dataCellStyle="Título 3"/>
-    <tableColumn id="7" xr3:uid="{86C55636-C35E-408D-9922-18CF7F29A89D}" name="Coeficiente de Variação" headerRowDxfId="3" dataDxfId="2" dataCellStyle="Título 3"/>
-    <tableColumn id="8" xr3:uid="{638FB161-8AF1-48E8-BF42-7B0824BB67BB}" name="Variância Amostral" headerRowDxfId="1" dataDxfId="0" dataCellStyle="Título 3"/>
+    <tableColumn id="5" xr3:uid="{CA7852E6-72C8-4A1E-95CB-43E78C3FC0C2}" name="Desvio Padrão" headerRowDxfId="7" dataDxfId="0" dataCellStyle="Título 3"/>
+    <tableColumn id="6" xr3:uid="{27646C93-0C02-40E2-85AE-D3CFA65AB91D}" name="Variância Populacional" headerRowDxfId="6" dataDxfId="5" dataCellStyle="Título 3"/>
+    <tableColumn id="7" xr3:uid="{86C55636-C35E-408D-9922-18CF7F29A89D}" name="Coeficiente de Variação" headerRowDxfId="4" dataDxfId="3" dataCellStyle="Título 3"/>
+    <tableColumn id="8" xr3:uid="{638FB161-8AF1-48E8-BF42-7B0824BB67BB}" name="Variância Amostral" headerRowDxfId="2" dataDxfId="1" dataCellStyle="Título 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1462,7 +1462,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" activeCellId="5" sqref="C18 D18 E18 F18 G18 H18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1470,7 @@
     <col min="1" max="1" width="10.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="7" customWidth="1"/>
     <col min="6" max="6" width="23.140625" customWidth="1"/>
     <col min="7" max="7" width="24.140625" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="E1" s="6"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="3"/>
@@ -1513,9 +1513,7 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="E3" s="6"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="3"/>
@@ -1529,7 +1527,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="3"/>
@@ -1543,7 +1541,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="3"/>
@@ -1557,7 +1555,7 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="3"/>
@@ -1571,7 +1569,7 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="3"/>
@@ -1585,7 +1583,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="3"/>
@@ -1599,7 +1597,7 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="3"/>
@@ -1613,7 +1611,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="3"/>
@@ -1627,7 +1625,7 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
@@ -1641,7 +1639,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="6"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="3"/>
@@ -1655,7 +1653,7 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="6"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="3"/>
@@ -1669,7 +1667,7 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="3"/>
@@ -1683,7 +1681,7 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
@@ -1697,7 +1695,7 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="3"/>
@@ -1711,7 +1709,7 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="3"/>
@@ -1731,7 +1729,7 @@
         <f>AVEDEV(B1:B18)</f>
         <v>467.55555555555537</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="6">
         <f>_xlfn.STDEV.P(B1:B18)</f>
         <v>513.49970848802229</v>
       </c>

</xml_diff>